<commit_message>
Carga de Archivo Excel
Ajuste de Ingreso Camion
</commit_message>
<xml_diff>
--- a/Test Data/Carga de Datos - Flujo Viaje.xlsx
+++ b/Test Data/Carga de Datos - Flujo Viaje.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\git\QA_ANCAP\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="7020"/>
+    <workbookView windowHeight="7020" windowWidth="9870" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
   <si>
     <t>URLLogin</t>
   </si>
@@ -110,9 +110,6 @@
     <t>ProdTransito</t>
   </si>
   <si>
-    <t>ProdTemperatura</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -132,12 +129,43 @@
   </si>
   <si>
     <t>Status TestCase</t>
+  </si>
+  <si>
+    <t>PROD NEGROS DISTRIBUIDORAS</t>
+  </si>
+  <si>
+    <t>KGR</t>
+  </si>
+  <si>
+    <t>TRANSFERENCIAS INTER PLANTA</t>
+  </si>
+  <si>
+    <t>PROD BLANCOS DISTRIBUIDORAS</t>
+  </si>
+  <si>
+    <t>ProdTempCargad</t>
+  </si>
+  <si>
+    <t>ProdTempLiquid</t>
+  </si>
+  <si>
+    <t>1817934</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>1817935</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -211,26 +239,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
       <color rgb="FFF3F6FB"/>
@@ -253,10 +281,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -291,7 +319,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,7 +354,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,21 +448,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -451,7 +479,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -503,40 +531,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="58.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -601,19 +631,22 @@
         <v>27</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="6" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -624,7 +657,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>180621</v>
+        <v>270621</v>
       </c>
       <c r="E2">
         <v>22</v>
@@ -645,7 +678,7 @@
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2">
         <v>691</v>
@@ -663,19 +696,19 @@
         <v>24</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T2" t="s">
         <v>25</v>
       </c>
       <c r="U2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V2" t="s">
         <v>23</v>
@@ -683,8 +716,17 @@
       <c r="W2">
         <v>16</v>
       </c>
+      <c r="X2">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -695,7 +737,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>180621</v>
+        <v>270621</v>
       </c>
       <c r="E3">
         <v>14</v>
@@ -716,13 +758,13 @@
         <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3">
         <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N3">
         <v>40013</v>
@@ -740,13 +782,13 @@
         <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
         <v>25</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V3" t="s">
         <v>23</v>
@@ -754,8 +796,17 @@
       <c r="W3">
         <v>16</v>
       </c>
+      <c r="X3">
+        <v>16</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -766,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>180621</v>
+        <v>270621</v>
       </c>
       <c r="E4">
         <v>14</v>
@@ -793,7 +844,7 @@
         <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4">
         <v>40013</v>
@@ -805,34 +856,262 @@
         <v>24</v>
       </c>
       <c r="Q4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R4" t="s">
         <v>25</v>
       </c>
       <c r="S4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T4" t="s">
         <v>25</v>
       </c>
       <c r="U4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W4">
         <v>16</v>
+      </c>
+      <c r="X4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>270621</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>733</v>
+      </c>
+      <c r="G5">
+        <v>43753294</v>
+      </c>
+      <c r="H5">
+        <v>3452609</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>803</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5">
+        <v>50010</v>
+      </c>
+      <c r="O5">
+        <v>400</v>
+      </c>
+      <c r="P5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" t="s">
+        <v>28</v>
+      </c>
+      <c r="V5" t="s">
+        <v>23</v>
+      </c>
+      <c r="W5">
+        <v>13</v>
+      </c>
+      <c r="X5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>270621</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>12993</v>
+      </c>
+      <c r="G6">
+        <v>25930036</v>
+      </c>
+      <c r="H6">
+        <v>6422108</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <v>60279</v>
+      </c>
+      <c r="O6">
+        <v>500</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U6" t="s">
+        <v>28</v>
+      </c>
+      <c r="V6" t="s">
+        <v>30</v>
+      </c>
+      <c r="W6">
+        <v>20</v>
+      </c>
+      <c r="X6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>270621</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>157</v>
+      </c>
+      <c r="G7">
+        <v>15965253</v>
+      </c>
+      <c r="H7">
+        <v>5920100</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>31</v>
+      </c>
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7">
+        <v>30017</v>
+      </c>
+      <c r="O7">
+        <v>600</v>
+      </c>
+      <c r="P7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U7" t="s">
+        <v>28</v>
+      </c>
+      <c r="V7" t="s">
+        <v>30</v>
+      </c>
+      <c r="W7">
+        <v>19</v>
+      </c>
+      <c r="X7">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="A4"/>
+    <hyperlink r:id="rId2" ref="A2"/>
+    <hyperlink r:id="rId3" ref="A3"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink r:id="rId6" ref="A7"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId4"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967294" orientation="portrait" paperSize="9" r:id="rId7" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>